<commit_message>
fix: compare_results and evaluates files
</commit_message>
<xml_diff>
--- a/assets/default_corpus/model_type_one/evaluate 1.xlsx
+++ b/assets/default_corpus/model_type_one/evaluate 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUJAE\DeepLearning\Software Required\Parser Proyect\assets\default_corpus\model_type_one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66A26AD-1ED9-462B-8617-FE5B8AF612D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8AF6BC-BB9E-4200-8691-D9C3798B7E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Ave 243 92A08 entre 92A y 94 La Cumbre San Miguel Del Padron La Habana</t>
   </si>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,6 +238,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,265 +553,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04EBE9F-E917-492C-AF6B-0ED5EB213D61}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="123.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="123.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
evaluate 1.xlsx now with 100 postal address
</commit_message>
<xml_diff>
--- a/assets/default_corpus/model_type_one/evaluate 1.xlsx
+++ b/assets/default_corpus/model_type_one/evaluate 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUJAE\DeepLearning\Software Required\Parser Proyect\assets\default_corpus\model_type_one\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUJAE\DeepLearning\Software Required\Parser Project\assets\default_corpus\model_type_one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8AF6BC-BB9E-4200-8691-D9C3798B7E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D210519C-4E31-46A0-BA96-C6F47BAAE565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
+    <workbookView xWindow="6108" yWindow="2268" windowWidth="17280" windowHeight="9420" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Ave 243 92A08 entre 92A y 94 La Cumbre San Miguel Del Padron La Habana</t>
   </si>
@@ -178,13 +178,169 @@
   </si>
   <si>
     <t>Avenida 45 10621 entre 106 y 108 Marianao La Habana</t>
+  </si>
+  <si>
+    <t>Pliar SN  e/  Julio de Cardenas y Lindero, Arroyo Naranjo, La Habana</t>
+  </si>
+  <si>
+    <t>31 A e/ 320 y 322, La Lisa, La Habana</t>
+  </si>
+  <si>
+    <t>C  e/  Delicias y San Francisco, San  Miguel del Padron, La Habana</t>
+  </si>
+  <si>
+    <t>39 e/ San Juan Bautista y Union, Plaza de la Revolucion, La Habana</t>
+  </si>
+  <si>
+    <t>Línea e/ 20 y 22, Vedado, Plaza de la Revolucion, La Habana</t>
+  </si>
+  <si>
+    <t>1ra e/ D y E, reparto Luyano Moderno, San  Miguel del Padron, La Habana</t>
+  </si>
+  <si>
+    <t>29 e/ 310 y 312, La Lisa, La Habana</t>
+  </si>
+  <si>
+    <t>428 e/ 19 y 21, Pena altas, Guanabo, La Habana del Este, La Habana</t>
+  </si>
+  <si>
+    <t>246 e/ 33 C y 35, La Lisa, La Habana</t>
+  </si>
+  <si>
+    <t>Figura e/ Vives y Esperanza, La Habana Vieja, La Habana</t>
+  </si>
+  <si>
+    <t>B e/ 1 y 2, Mercedita, San Miguel del Padron, La Habana</t>
+  </si>
+  <si>
+    <t>161 e/ 310 y 314, Valle Brande, La Lisa, La Habana</t>
+  </si>
+  <si>
+    <t>Santa Ana e/ Luco y Villanueva, Diez de Octubre, La Habana</t>
+  </si>
+  <si>
+    <t>44 e/ 19 Y  21, Playa, La Habana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Joaquin Delgado e Santa Clara y Esperanza, reparto Parraga, Arroyo Naranjo, La Habana</t>
+  </si>
+  <si>
+    <t>CALLE C  # 9512 A  /  6 y 10 Reparto Altahabana ,BOYEROS,La Habana</t>
+  </si>
+  <si>
+    <t>Calle 160 No 4509E / Ave 45 y Ave 47,LA LISA,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Maceo  # 61 Alto entre Bertenati y Nazareno,PLAZA DE LA REVOLUCION,La Habana</t>
+  </si>
+  <si>
+    <t>Destramoes  # 58 entre Luis esteves y Lacret, Santo Suarez,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Máximo Gómez  # 264 Altos  E / 27 DE Noviembre y Pereira,REGLA,La Habana</t>
+  </si>
+  <si>
+    <t>Calle San Mariano  # 761 entre San Juan Bosco y Graciela apto 8, Vibora,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Calle 111 E / cALLE 24 y Calle 24 A Edificio 6 apt 4 Reparto Sierra Maestra,BOYEROS,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Barbería e /  Calle Universidad y Calle Estevez edf 32 apto 4,CERRO,La Habana</t>
+  </si>
+  <si>
+    <t>CALLE 18  #  505 BAJO ENTRE CONCEPCION Y SAN FRANCISCO LAWTON,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>180  #  42109 ENTRE 421 Y 423, LA AURORA,BOYEROS,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Gertrudis Oeste  # 459 E /  Anita y Goicuria Repto Sevillano,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Avenida Santa Catalina e / Mayia Rodriguez  y La Sola,Edificio 616,Apto 3,Reparto Santos Suarez,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Pinar  # 8003 E / Santa Teresa y Collazo,Reparto Ponce,ARROYO NARANJO,La Habana</t>
+  </si>
+  <si>
+    <t>Avenida Ciudamar  # 17521 e /  Calle 13 y Calle 15, Reparto Ciudamar,SAN MIGUEL DEL PADRON,La Habana</t>
+  </si>
+  <si>
+    <t>Calzada de 10 de Octubre  # 1155 apto 1 e /  Santa Catalina y San Mariano,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Calle 5ta B  #  9606 2 int,entre calle 96 y 98, Barrio Querejeta,PLAYA,La Habana</t>
+  </si>
+  <si>
+    <t>Calle 1 No  17416 E / Calle A y Calle San Luis,Reparto Encanto,SAN MIGUEL DEL PADRON,La Habana</t>
+  </si>
+  <si>
+    <t>Calle 9na  # 14 ,Apto 3 E / Calle E y Calle D,Barrio Lawton,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Calle Tenerifr # 156 apto  6 E /  Rastro y Carmen  ,CENTRO HABANA,La Habana</t>
+  </si>
+  <si>
+    <t>Ave Entrada E / Ave de los Ocujes y Ave  de la Ceiba Edificio 2 APTO 5 Reparto Santa Catalina,CERRO,La Habana</t>
+  </si>
+  <si>
+    <t>Sta Catalina e / Vento y San Juán Bosco ed 817 apto 4,DIEZ DE OCTUBRE,La Habana</t>
+  </si>
+  <si>
+    <t>Aliados e/ Pasaje D y Central, San Miguel del Padrón, La Habana</t>
+  </si>
+  <si>
+    <t>Estancia e/ San Pedro y Lombill, Nuevo Vedado, Plaza de la Revolucion, La Habana</t>
+  </si>
+  <si>
+    <t>Estrella e/ Aguila y Angeles, Centro Habana, La Habana</t>
+  </si>
+  <si>
+    <t>Virginia e/ Pinar del Rio y Woodbury, reparto Callejas, Arroyo Naranjo, La Habana</t>
+  </si>
+  <si>
+    <t>Recurso e/ Masarredo y Lindero, Nuevo Vedado, Plaza de la Revolucion, La Habana</t>
+  </si>
+  <si>
+    <t>San Quintin e/ Salvador y Cerezo, Cerro, La Habana</t>
+  </si>
+  <si>
+    <t>Calle 6ta entre 16 y 17 Edificio 37 Apto 29 Reparto Guiteras  LA HABANA DEL ESTE La Habana</t>
+  </si>
+  <si>
+    <t>Calle 308   1904A entre 19 y 21 Reparto Santa Fe  PLAYA La Habana</t>
+  </si>
+  <si>
+    <t>Calle Santa Rosa     8 e entre San Antonio y Rizo  PLaza PLAZA DE LA REVOLUCION La Habana</t>
+  </si>
+  <si>
+    <t>Calle 17    853 e entre  4 y 6 PLAZA DE LA REVOLUCION La Habana</t>
+  </si>
+  <si>
+    <t>67A No 11404 e 114 y 116 MARIANAO La Habana</t>
+  </si>
+  <si>
+    <t>Calle 203 entre 290 y Prensa Latina, Poblado Pueblo del Chico, BOYEROS, La Habana</t>
+  </si>
+  <si>
+    <t>A # 319/11 Y 12</t>
+  </si>
+  <si>
+    <t>REAL # 181</t>
+  </si>
+  <si>
+    <t>JACINTO ROY # 14 / ANGELITA Y BERENGUER, VIEJA LINDA</t>
+  </si>
+  <si>
+    <t>PUERTA CERRADA 222 / ALAMBIQUE Y FLORIDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +364,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -226,8 +389,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -238,10 +402,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E3D9C271-6CD3-4632-A432-0E876547704A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -553,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04EBE9F-E917-492C-AF6B-0ED5EB213D61}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,8 +973,265 @@
         <v>45</v>
       </c>
     </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
+      <c r="A51" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add: completa evaluates 1.xlsx with 100 real address
</commit_message>
<xml_diff>
--- a/assets/default_corpus/model_type_one/evaluate 1.xlsx
+++ b/assets/default_corpus/model_type_one/evaluate 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CUJAE\DeepLearning\Software Required\Parser Project\assets\default_corpus\model_type_one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D210519C-4E31-46A0-BA96-C6F47BAAE565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72644D5B-4102-4285-AA52-E91427D0568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="2268" windowWidth="17280" windowHeight="9420" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CE3A1A6B-7415-49B6-8F8D-6A02B855C26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Ave 243 92A08 entre 92A y 94 La Cumbre San Miguel Del Padron La Habana</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>PUERTA CERRADA 222 / ALAMBIQUE Y FLORIDA</t>
+  </si>
+  <si>
+    <t>7MA  # 10302 APT 18  E/ L Y K ALTAHABANA</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -403,6 +406,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04EBE9F-E917-492C-AF6B-0ED5EB213D61}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:A100"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,6 +1237,11 @@
         <v>99</v>
       </c>
     </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>